<commit_message>
push sementara untuk tampilan yayasan
</commit_message>
<xml_diff>
--- a/public/storage/simpanFile/daftar siswa-siswi TK.xlsx
+++ b/public/storage/simpanFile/daftar siswa-siswi TK.xlsx
@@ -1781,7 +1781,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:W119"/>
+  <dimension ref="A1:X119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="86" zoomScaleNormal="70" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E12" sqref="E12"/>
@@ -1814,7 +1814,7 @@
     <col min="23" max="23" width="8.88671875" customWidth="true" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" customHeight="1" ht="18">
+    <row r="1" spans="1:24" customHeight="1" ht="18">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1840,7 @@
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
     </row>
-    <row r="2" spans="1:23" customHeight="1" ht="18">
+    <row r="2" spans="1:24" customHeight="1" ht="18">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1866,7 +1866,7 @@
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
     </row>
-    <row r="3" spans="1:23" customHeight="1" ht="18">
+    <row r="3" spans="1:24" customHeight="1" ht="18">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1892,7 +1892,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
     </row>
-    <row r="4" spans="1:23" customHeight="1" ht="18">
+    <row r="4" spans="1:24" customHeight="1" ht="18">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1920,7 +1920,7 @@
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
     </row>
-    <row r="5" spans="1:23" customHeight="1" ht="17.4" s="2" customFormat="1">
+    <row r="5" spans="1:24" customHeight="1" ht="17.4" s="2" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -1983,11 +1983,11 @@
       <c r="V5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="6" spans="1:23" customHeight="1" ht="17.4" s="2" customFormat="1">
+    <row r="6" spans="1:24" customHeight="1" ht="17.4" s="2" customFormat="1">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2016,11 +2016,11 @@
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
       <c r="V6" s="7"/>
-      <c r="W6" s="2">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" customHeight="1" ht="18">
+      <c r="X6" s="2">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" customHeight="1" ht="18">
       <c r="A7" s="12">
         <v>9691</v>
       </c>
@@ -2077,11 +2077,11 @@
         <v>1</v>
       </c>
       <c r="V7" s="12"/>
-      <c r="W7">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" customHeight="1" ht="18">
+      <c r="X7">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" customHeight="1" ht="18">
       <c r="A8" s="12">
         <v>9692</v>
       </c>
@@ -2138,11 +2138,11 @@
         <v>1</v>
       </c>
       <c r="V8" s="12"/>
-      <c r="W8">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" customHeight="1" ht="18">
+      <c r="X8">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" customHeight="1" ht="18">
       <c r="A9" s="12">
         <v>9693</v>
       </c>
@@ -2199,11 +2199,11 @@
         <v>1</v>
       </c>
       <c r="V9" s="12"/>
-      <c r="W9">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" customHeight="1" ht="18">
+      <c r="X9">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" customHeight="1" ht="18">
       <c r="A10" s="12">
         <v>9694</v>
       </c>
@@ -2260,11 +2260,11 @@
         <v>1</v>
       </c>
       <c r="V10" s="12"/>
-      <c r="W10">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" customHeight="1" ht="18">
+      <c r="X10">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" customHeight="1" ht="18">
       <c r="A11" s="12">
         <v>9695</v>
       </c>
@@ -2321,11 +2321,11 @@
         <v>1</v>
       </c>
       <c r="V11" s="12"/>
-      <c r="W11">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" customHeight="1" ht="18">
+      <c r="X11">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" customHeight="1" ht="18">
       <c r="A12" s="12">
         <v>9696</v>
       </c>
@@ -2382,11 +2382,11 @@
         <v>1</v>
       </c>
       <c r="V12" s="12"/>
-      <c r="W12">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" customHeight="1" ht="18">
+      <c r="X12">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" customHeight="1" ht="18">
       <c r="A13" s="12">
         <v>9697</v>
       </c>
@@ -2443,11 +2443,11 @@
         <v>1</v>
       </c>
       <c r="V13" s="12"/>
-      <c r="W13">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" customHeight="1" ht="18">
+      <c r="X13">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" customHeight="1" ht="18">
       <c r="A14" s="12">
         <v>9698</v>
       </c>
@@ -2504,11 +2504,11 @@
         <v>1</v>
       </c>
       <c r="V14" s="12"/>
-      <c r="W14">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" customHeight="1" ht="18">
+      <c r="X14">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" customHeight="1" ht="18">
       <c r="A15" s="12">
         <v>9699</v>
       </c>
@@ -2565,11 +2565,11 @@
         <v>1</v>
       </c>
       <c r="V15" s="12"/>
-      <c r="W15">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" customHeight="1" ht="18">
+      <c r="X15">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" customHeight="1" ht="18">
       <c r="A16" s="12">
         <v>9700</v>
       </c>
@@ -2626,11 +2626,11 @@
         <v>1</v>
       </c>
       <c r="V16" s="12"/>
-      <c r="W16">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" customHeight="1" ht="18">
+      <c r="X16">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" customHeight="1" ht="18">
       <c r="A17" s="12">
         <v>9701</v>
       </c>
@@ -2687,11 +2687,11 @@
         <v>1</v>
       </c>
       <c r="V17" s="12"/>
-      <c r="W17">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" customHeight="1" ht="18">
+      <c r="X17">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" customHeight="1" ht="18">
       <c r="A18" s="12">
         <v>9702</v>
       </c>
@@ -2748,11 +2748,11 @@
         <v>1</v>
       </c>
       <c r="V18" s="12"/>
-      <c r="W18">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" customHeight="1" ht="18">
+      <c r="X18">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" customHeight="1" ht="18">
       <c r="A19" s="12">
         <v>9703</v>
       </c>
@@ -2809,11 +2809,11 @@
         <v>1</v>
       </c>
       <c r="V19" s="12"/>
-      <c r="W19">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" customHeight="1" ht="18">
+      <c r="X19">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" customHeight="1" ht="18">
       <c r="A20" s="12">
         <v>9704</v>
       </c>
@@ -2870,11 +2870,11 @@
         <v>1</v>
       </c>
       <c r="V20" s="12"/>
-      <c r="W20">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" customHeight="1" ht="18">
+      <c r="X20">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" customHeight="1" ht="18">
       <c r="A21" s="12">
         <v>9705</v>
       </c>
@@ -2931,11 +2931,11 @@
         <v>1</v>
       </c>
       <c r="V21" s="12"/>
-      <c r="W21">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" customHeight="1" ht="18">
+      <c r="X21">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" customHeight="1" ht="18">
       <c r="A22" s="12">
         <v>9706</v>
       </c>
@@ -2992,11 +2992,11 @@
         <v>1</v>
       </c>
       <c r="V22" s="12"/>
-      <c r="W22">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" customHeight="1" ht="18">
+      <c r="X22">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" customHeight="1" ht="18">
       <c r="A23" s="12">
         <v>9707</v>
       </c>
@@ -3051,11 +3051,11 @@
         <v>1</v>
       </c>
       <c r="V23" s="12"/>
-      <c r="W23">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" customHeight="1" ht="18">
+      <c r="X23">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" customHeight="1" ht="18">
       <c r="A24" s="12">
         <v>9708</v>
       </c>
@@ -3112,11 +3112,11 @@
         <v>1</v>
       </c>
       <c r="V24" s="12"/>
-      <c r="W24">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" customHeight="1" ht="18">
+      <c r="X24">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" customHeight="1" ht="18">
       <c r="A25" s="12">
         <v>9709</v>
       </c>
@@ -3173,11 +3173,11 @@
         <v>1</v>
       </c>
       <c r="V25" s="12"/>
-      <c r="W25">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" customHeight="1" ht="18">
+      <c r="X25">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" customHeight="1" ht="18">
       <c r="A26" s="12">
         <v>9710</v>
       </c>
@@ -3234,11 +3234,11 @@
         <v>1</v>
       </c>
       <c r="V26" s="12"/>
-      <c r="W26">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" customHeight="1" ht="18">
+      <c r="X26">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" customHeight="1" ht="18">
       <c r="A27" s="12">
         <v>9711</v>
       </c>
@@ -3295,11 +3295,11 @@
         <v>1</v>
       </c>
       <c r="V27" s="12"/>
-      <c r="W27">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" customHeight="1" ht="18">
+      <c r="X27">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" customHeight="1" ht="18">
       <c r="A28" s="12">
         <v>9712</v>
       </c>
@@ -3356,11 +3356,11 @@
         <v>1</v>
       </c>
       <c r="V28" s="12"/>
-      <c r="W28">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" customHeight="1" ht="18">
+      <c r="X28">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" customHeight="1" ht="18">
       <c r="A29" s="12">
         <v>9713</v>
       </c>
@@ -3417,11 +3417,11 @@
         <v>1</v>
       </c>
       <c r="V29" s="12"/>
-      <c r="W29">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" customHeight="1" ht="18">
+      <c r="X29">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" customHeight="1" ht="18">
       <c r="A30" s="12">
         <v>9714</v>
       </c>
@@ -3478,11 +3478,11 @@
         <v>1</v>
       </c>
       <c r="V30" s="12"/>
-      <c r="W30">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" customHeight="1" ht="18">
+      <c r="X30">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" customHeight="1" ht="18">
       <c r="A31" s="12">
         <v>9715</v>
       </c>
@@ -3539,11 +3539,11 @@
         <v>1</v>
       </c>
       <c r="V31" s="12"/>
-      <c r="W31">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" customHeight="1" ht="18">
+      <c r="X31">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" customHeight="1" ht="18">
       <c r="A32" s="12">
         <v>9716</v>
       </c>
@@ -3598,11 +3598,11 @@
         <v>1</v>
       </c>
       <c r="V32" s="12"/>
-      <c r="W32">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" customHeight="1" ht="18">
+      <c r="X32">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" customHeight="1" ht="18">
       <c r="A33" s="12">
         <v>9717</v>
       </c>
@@ -3659,11 +3659,11 @@
         <v>1</v>
       </c>
       <c r="V33" s="12"/>
-      <c r="W33">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" customHeight="1" ht="18">
+      <c r="X33">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" customHeight="1" ht="18">
       <c r="A34" s="12">
         <v>9718</v>
       </c>
@@ -3718,11 +3718,11 @@
         <v>1</v>
       </c>
       <c r="V34" s="12"/>
-      <c r="W34">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" customHeight="1" ht="18">
+      <c r="X34">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" customHeight="1" ht="18">
       <c r="A35" s="12">
         <v>9719</v>
       </c>
@@ -3779,11 +3779,11 @@
         <v>1</v>
       </c>
       <c r="V35" s="12"/>
-      <c r="W35">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" customHeight="1" ht="18">
+      <c r="X35">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" customHeight="1" ht="18">
       <c r="A36" s="12">
         <v>9720</v>
       </c>
@@ -3840,11 +3840,11 @@
         <v>1</v>
       </c>
       <c r="V36" s="12"/>
-      <c r="W36">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" customHeight="1" ht="18">
+      <c r="X36">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" customHeight="1" ht="18">
       <c r="A37" s="12">
         <v>9721</v>
       </c>
@@ -3901,11 +3901,11 @@
         <v>1</v>
       </c>
       <c r="V37" s="12"/>
-      <c r="W37">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" customHeight="1" ht="18">
+      <c r="X37">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" customHeight="1" ht="18">
       <c r="A38" s="12">
         <v>9722</v>
       </c>
@@ -3962,11 +3962,11 @@
         <v>1</v>
       </c>
       <c r="V38" s="12"/>
-      <c r="W38">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" customHeight="1" ht="18">
+      <c r="X38">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" customHeight="1" ht="18">
       <c r="A39" s="12">
         <v>9723</v>
       </c>
@@ -4021,11 +4021,11 @@
         <v>1</v>
       </c>
       <c r="V39" s="12"/>
-      <c r="W39">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" customHeight="1" ht="18">
+      <c r="X39">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" customHeight="1" ht="18">
       <c r="A40" s="12">
         <v>9724</v>
       </c>
@@ -4082,11 +4082,11 @@
         <v>1</v>
       </c>
       <c r="V40" s="12"/>
-      <c r="W40">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" customHeight="1" ht="18">
+      <c r="X40">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" customHeight="1" ht="18">
       <c r="A41" s="12">
         <v>9725</v>
       </c>
@@ -4143,11 +4143,11 @@
         <v>1</v>
       </c>
       <c r="V41" s="12"/>
-      <c r="W41">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" customHeight="1" ht="18">
+      <c r="X41">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" customHeight="1" ht="18">
       <c r="A42" s="12">
         <v>9726</v>
       </c>
@@ -4204,11 +4204,11 @@
         <v>1</v>
       </c>
       <c r="V42" s="12"/>
-      <c r="W42">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" customHeight="1" ht="18">
+      <c r="X42">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" customHeight="1" ht="18">
       <c r="A43" s="12">
         <v>9727</v>
       </c>
@@ -4263,11 +4263,11 @@
         <v>1</v>
       </c>
       <c r="V43" s="12"/>
-      <c r="W43">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" customHeight="1" ht="18">
+      <c r="X43">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" customHeight="1" ht="18">
       <c r="A44" s="12">
         <v>9728</v>
       </c>
@@ -4322,11 +4322,11 @@
         <v>1</v>
       </c>
       <c r="V44" s="12"/>
-      <c r="W44">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" customHeight="1" ht="18">
+      <c r="X44">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" customHeight="1" ht="18">
       <c r="A45" s="12">
         <v>9729</v>
       </c>
@@ -4383,11 +4383,11 @@
         <v>1</v>
       </c>
       <c r="V45" s="12"/>
-      <c r="W45">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" customHeight="1" ht="18">
+      <c r="X45">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" customHeight="1" ht="18">
       <c r="A46" s="12">
         <v>9730</v>
       </c>
@@ -4444,11 +4444,11 @@
         <v>1</v>
       </c>
       <c r="V46" s="12"/>
-      <c r="W46">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" customHeight="1" ht="18">
+      <c r="X46">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" customHeight="1" ht="18">
       <c r="A47" s="12">
         <v>9731</v>
       </c>
@@ -4505,11 +4505,11 @@
         <v>1</v>
       </c>
       <c r="V47" s="12"/>
-      <c r="W47">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" customHeight="1" ht="18">
+      <c r="X47">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" customHeight="1" ht="18">
       <c r="A48" s="12">
         <v>9732</v>
       </c>
@@ -4566,11 +4566,11 @@
         <v>1</v>
       </c>
       <c r="V48" s="12"/>
-      <c r="W48">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" customHeight="1" ht="18">
+      <c r="X48">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" customHeight="1" ht="18">
       <c r="A49" s="12">
         <v>9733</v>
       </c>
@@ -4627,11 +4627,11 @@
         <v>1</v>
       </c>
       <c r="V49" s="12"/>
-      <c r="W49">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="50" spans="1:23" customHeight="1" ht="18">
+      <c r="X49">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" customHeight="1" ht="18">
       <c r="A50" s="12">
         <v>9734</v>
       </c>
@@ -4682,11 +4682,11 @@
         <v>1</v>
       </c>
       <c r="V50" s="12"/>
-      <c r="W50">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="51" spans="1:23" customHeight="1" ht="18">
+      <c r="X50">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" customHeight="1" ht="18">
       <c r="A51" s="12">
         <v>9735</v>
       </c>
@@ -4739,11 +4739,11 @@
         <v>1</v>
       </c>
       <c r="V51" s="12"/>
-      <c r="W51">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="52" spans="1:23" customHeight="1" ht="18">
+      <c r="X51">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" customHeight="1" ht="18">
       <c r="A52" s="12">
         <v>9736</v>
       </c>
@@ -4796,11 +4796,11 @@
         <v>1</v>
       </c>
       <c r="V52" s="12"/>
-      <c r="W52">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="53" spans="1:23" customHeight="1" ht="18">
+      <c r="X52">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" customHeight="1" ht="18">
       <c r="A53" s="12">
         <v>9737</v>
       </c>
@@ -4853,11 +4853,11 @@
         <v>1</v>
       </c>
       <c r="V53" s="12"/>
-      <c r="W53">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="54" spans="1:23" customHeight="1" ht="18">
+      <c r="X53">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" customHeight="1" ht="18">
       <c r="A54" s="12">
         <v>9738</v>
       </c>
@@ -4910,11 +4910,11 @@
         <v>1</v>
       </c>
       <c r="V54" s="12"/>
-      <c r="W54">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="55" spans="1:23" customHeight="1" ht="18">
+      <c r="X54">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" customHeight="1" ht="18">
       <c r="A55" s="12">
         <v>9739</v>
       </c>
@@ -4965,11 +4965,11 @@
         <v>1</v>
       </c>
       <c r="V55" s="12"/>
-      <c r="W55">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="56" spans="1:23" customHeight="1" ht="18">
+      <c r="X55">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" customHeight="1" ht="18">
       <c r="A56" s="12">
         <v>9740</v>
       </c>
@@ -5022,11 +5022,11 @@
         <v>1</v>
       </c>
       <c r="V56" s="12"/>
-      <c r="W56">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="57" spans="1:23" customHeight="1" ht="18">
+      <c r="X56">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" customHeight="1" ht="18">
       <c r="A57" s="12">
         <v>9741</v>
       </c>
@@ -5079,11 +5079,11 @@
         <v>1</v>
       </c>
       <c r="V57" s="12"/>
-      <c r="W57">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="58" spans="1:23" customHeight="1" ht="18">
+      <c r="X57">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" customHeight="1" ht="18">
       <c r="A58" s="12">
         <v>9742</v>
       </c>
@@ -5136,11 +5136,11 @@
         <v>1</v>
       </c>
       <c r="V58" s="12"/>
-      <c r="W58">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" customHeight="1" ht="18">
+      <c r="X58">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" customHeight="1" ht="18">
       <c r="A59" s="12">
         <v>9743</v>
       </c>
@@ -5193,11 +5193,11 @@
         <v>1</v>
       </c>
       <c r="V59" s="12"/>
-      <c r="W59">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" customHeight="1" ht="18">
+      <c r="X59">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" customHeight="1" ht="18">
       <c r="A60" s="12">
         <v>9744</v>
       </c>
@@ -5252,11 +5252,11 @@
         <v>1</v>
       </c>
       <c r="V60" s="12"/>
-      <c r="W60">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" customHeight="1" ht="18">
+      <c r="X60">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" customHeight="1" ht="18">
       <c r="A61" s="12">
         <v>9745</v>
       </c>
@@ -5309,11 +5309,11 @@
         <v>1</v>
       </c>
       <c r="V61" s="12"/>
-      <c r="W61">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="62" spans="1:23" customHeight="1" ht="18">
+      <c r="X61">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" customHeight="1" ht="18">
       <c r="A62" s="12">
         <v>9746</v>
       </c>
@@ -5366,11 +5366,11 @@
         <v>1</v>
       </c>
       <c r="V62" s="12"/>
-      <c r="W62">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="63" spans="1:23" customHeight="1" ht="18">
+      <c r="X62">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" customHeight="1" ht="18">
       <c r="A63" s="12">
         <v>9747</v>
       </c>
@@ -5425,11 +5425,11 @@
         <v>1</v>
       </c>
       <c r="V63" s="12"/>
-      <c r="W63">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" customHeight="1" ht="18">
+      <c r="X63">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" customHeight="1" ht="18">
       <c r="A64" s="12">
         <v>9748</v>
       </c>
@@ -5484,11 +5484,11 @@
         <v>1</v>
       </c>
       <c r="V64" s="12"/>
-      <c r="W64">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" customHeight="1" ht="18">
+      <c r="X64">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" customHeight="1" ht="18">
       <c r="A65" s="12">
         <v>9749</v>
       </c>
@@ -5541,11 +5541,11 @@
         <v>1</v>
       </c>
       <c r="V65" s="12"/>
-      <c r="W65">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="66" spans="1:23" customHeight="1" ht="18">
+      <c r="X65">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" customHeight="1" ht="18">
       <c r="A66" s="12">
         <v>9750</v>
       </c>
@@ -5600,11 +5600,11 @@
         <v>1</v>
       </c>
       <c r="V66" s="12"/>
-      <c r="W66">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23" customHeight="1" ht="18">
+      <c r="X66">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" customHeight="1" ht="18">
       <c r="A67" s="12">
         <v>9751</v>
       </c>
@@ -5657,11 +5657,11 @@
         <v>1</v>
       </c>
       <c r="V67" s="12"/>
-      <c r="W67">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23" customHeight="1" ht="18">
+      <c r="X67">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" customHeight="1" ht="18">
       <c r="A68" s="12">
         <v>9752</v>
       </c>
@@ -5714,11 +5714,11 @@
         <v>1</v>
       </c>
       <c r="V68" s="12"/>
-      <c r="W68">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="69" spans="1:23" customHeight="1" ht="18">
+      <c r="X68">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" customHeight="1" ht="18">
       <c r="A69" s="12">
         <v>9753</v>
       </c>
@@ -5771,11 +5771,11 @@
         <v>1</v>
       </c>
       <c r="V69" s="12"/>
-      <c r="W69">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="70" spans="1:23" customHeight="1" ht="18">
+      <c r="X69">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" customHeight="1" ht="18">
       <c r="A70" s="12">
         <v>9754</v>
       </c>
@@ -5828,11 +5828,11 @@
         <v>1</v>
       </c>
       <c r="V70" s="12"/>
-      <c r="W70">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="71" spans="1:23" customHeight="1" ht="18">
+      <c r="X70">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" customHeight="1" ht="18">
       <c r="A71" s="12">
         <v>9755</v>
       </c>
@@ -5885,11 +5885,11 @@
         <v>1</v>
       </c>
       <c r="V71" s="12"/>
-      <c r="W71">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="72" spans="1:23" customHeight="1" ht="18">
+      <c r="X71">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" customHeight="1" ht="18">
       <c r="A72" s="12">
         <v>9756</v>
       </c>
@@ -5942,11 +5942,11 @@
         <v>1</v>
       </c>
       <c r="V72" s="12"/>
-      <c r="W72">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="73" spans="1:23" customHeight="1" ht="18">
+      <c r="X72">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" customHeight="1" ht="18">
       <c r="A73" s="12">
         <v>9757</v>
       </c>
@@ -5997,11 +5997,11 @@
         <v>1</v>
       </c>
       <c r="V73" s="12"/>
-      <c r="W73">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="74" spans="1:23" customHeight="1" ht="18">
+      <c r="X73">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" customHeight="1" ht="18">
       <c r="A74" s="12">
         <v>9758</v>
       </c>
@@ -6052,11 +6052,11 @@
         <v>1</v>
       </c>
       <c r="V74" s="12"/>
-      <c r="W74">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="75" spans="1:23" customHeight="1" ht="18">
+      <c r="X74">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" customHeight="1" ht="18">
       <c r="A75" s="12">
         <v>9759</v>
       </c>
@@ -6107,11 +6107,11 @@
         <v>1</v>
       </c>
       <c r="V75" s="12"/>
-      <c r="W75">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="76" spans="1:23" customHeight="1" ht="18">
+      <c r="X75">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" customHeight="1" ht="18">
       <c r="A76" s="12">
         <v>9760</v>
       </c>
@@ -6164,11 +6164,11 @@
         <v>1</v>
       </c>
       <c r="V76" s="12"/>
-      <c r="W76">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="77" spans="1:23" customHeight="1" ht="18">
+      <c r="X76">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" customHeight="1" ht="18">
       <c r="A77" s="12">
         <v>9761</v>
       </c>
@@ -6221,11 +6221,11 @@
         <v>1</v>
       </c>
       <c r="V77" s="12"/>
-      <c r="W77">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="78" spans="1:23" customHeight="1" ht="18">
+      <c r="X77">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" customHeight="1" ht="18">
       <c r="A78" s="12">
         <v>9762</v>
       </c>
@@ -6278,11 +6278,11 @@
         <v>1</v>
       </c>
       <c r="V78" s="12"/>
-      <c r="W78">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="79" spans="1:23" customHeight="1" ht="18">
+      <c r="X78">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" customHeight="1" ht="18">
       <c r="A79" s="12">
         <v>9763</v>
       </c>
@@ -6335,11 +6335,11 @@
         <v>1</v>
       </c>
       <c r="V79" s="12"/>
-      <c r="W79">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="80" spans="1:23" customHeight="1" ht="18">
+      <c r="X79">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" customHeight="1" ht="18">
       <c r="A80" s="12">
         <v>9764</v>
       </c>
@@ -6392,11 +6392,11 @@
         <v>1</v>
       </c>
       <c r="V80" s="12"/>
-      <c r="W80">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="81" spans="1:23" customHeight="1" ht="18">
+      <c r="X80">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" customHeight="1" ht="18">
       <c r="A81" s="12">
         <v>9765</v>
       </c>
@@ -6447,11 +6447,11 @@
         <v>1</v>
       </c>
       <c r="V81" s="12"/>
-      <c r="W81">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="82" spans="1:23" customHeight="1" ht="18">
+      <c r="X81">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="82" spans="1:24" customHeight="1" ht="18">
       <c r="A82" s="12">
         <v>9766</v>
       </c>
@@ -6504,11 +6504,11 @@
         <v>1</v>
       </c>
       <c r="V82" s="12"/>
-      <c r="W82">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="83" spans="1:23" customHeight="1" ht="18">
+      <c r="X82">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="83" spans="1:24" customHeight="1" ht="18">
       <c r="A83" s="12">
         <v>9767</v>
       </c>
@@ -6561,11 +6561,11 @@
         <v>1</v>
       </c>
       <c r="V83" s="12"/>
-      <c r="W83">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="84" spans="1:23" customHeight="1" ht="18">
+      <c r="X83">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" customHeight="1" ht="18">
       <c r="A84" s="12">
         <v>9768</v>
       </c>
@@ -6618,11 +6618,11 @@
         <v>1</v>
       </c>
       <c r="V84" s="12"/>
-      <c r="W84">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="85" spans="1:23" customHeight="1" ht="18">
+      <c r="X84">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" customHeight="1" ht="18">
       <c r="A85" s="12">
         <v>9769</v>
       </c>
@@ -6675,11 +6675,11 @@
         <v>1</v>
       </c>
       <c r="V85" s="12"/>
-      <c r="W85">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="86" spans="1:23" customHeight="1" ht="18">
+      <c r="X85">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" customHeight="1" ht="18">
       <c r="A86" s="12">
         <v>9770</v>
       </c>
@@ -6732,11 +6732,11 @@
         <v>1</v>
       </c>
       <c r="V86" s="12"/>
-      <c r="W86">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="87" spans="1:23" customHeight="1" ht="18">
+      <c r="X86">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" customHeight="1" ht="18">
       <c r="A87" s="12">
         <v>9771</v>
       </c>
@@ -6789,11 +6789,11 @@
         <v>1</v>
       </c>
       <c r="V87" s="12"/>
-      <c r="W87">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="88" spans="1:23" customHeight="1" ht="18">
+      <c r="X87">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" customHeight="1" ht="18">
       <c r="A88" s="12">
         <v>9772</v>
       </c>
@@ -6846,11 +6846,11 @@
         <v>1</v>
       </c>
       <c r="V88" s="12"/>
-      <c r="W88">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="89" spans="1:23" customHeight="1" ht="18">
+      <c r="X88">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" customHeight="1" ht="18">
       <c r="A89" s="12">
         <v>9773</v>
       </c>
@@ -6903,11 +6903,11 @@
         <v>1</v>
       </c>
       <c r="V89" s="12"/>
-      <c r="W89">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="90" spans="1:23" customHeight="1" ht="18">
+      <c r="X89">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" customHeight="1" ht="18">
       <c r="A90" s="12">
         <v>9774</v>
       </c>
@@ -6960,11 +6960,11 @@
         <v>1</v>
       </c>
       <c r="V90" s="12"/>
-      <c r="W90">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="91" spans="1:23" customHeight="1" ht="18">
+      <c r="X90">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" customHeight="1" ht="18">
       <c r="A91" s="12">
         <v>9775</v>
       </c>
@@ -7017,11 +7017,11 @@
         <v>1</v>
       </c>
       <c r="V91" s="12"/>
-      <c r="W91">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="92" spans="1:23" customHeight="1" ht="18">
+      <c r="X91">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" customHeight="1" ht="18">
       <c r="A92" s="12">
         <v>9776</v>
       </c>
@@ -7074,11 +7074,11 @@
         <v>1</v>
       </c>
       <c r="V92" s="12"/>
-      <c r="W92">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="93" spans="1:23" customHeight="1" ht="18">
+      <c r="X92">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" customHeight="1" ht="18">
       <c r="A93" s="12">
         <v>9777</v>
       </c>
@@ -7131,11 +7131,11 @@
         <v>1</v>
       </c>
       <c r="V93" s="12"/>
-      <c r="W93">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="94" spans="1:23" customHeight="1" ht="18">
+      <c r="X93">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" customHeight="1" ht="18">
       <c r="A94" s="12">
         <v>9778</v>
       </c>
@@ -7188,11 +7188,11 @@
         <v>1</v>
       </c>
       <c r="V94" s="12"/>
-      <c r="W94">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="95" spans="1:23" customHeight="1" ht="18">
+      <c r="X94">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" customHeight="1" ht="18">
       <c r="A95" s="12">
         <v>9779</v>
       </c>
@@ -7245,11 +7245,11 @@
         <v>1</v>
       </c>
       <c r="V95" s="12"/>
-      <c r="W95">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="96" spans="1:23" customHeight="1" ht="18">
+      <c r="X95">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" customHeight="1" ht="18">
       <c r="A96" s="12">
         <v>9780</v>
       </c>
@@ -7302,11 +7302,11 @@
         <v>1</v>
       </c>
       <c r="V96" s="12"/>
-      <c r="W96">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="97" spans="1:23" customHeight="1" ht="18">
+      <c r="X96">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" customHeight="1" ht="18">
       <c r="A97" s="12">
         <v>9781</v>
       </c>
@@ -7357,11 +7357,11 @@
         <v>1</v>
       </c>
       <c r="V97" s="12"/>
-      <c r="W97">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="98" spans="1:23" customHeight="1" ht="18">
+      <c r="X97">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" customHeight="1" ht="18">
       <c r="A98" s="12">
         <v>9782</v>
       </c>
@@ -7412,11 +7412,11 @@
         <v>1</v>
       </c>
       <c r="V98" s="12"/>
-      <c r="W98">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="99" spans="1:23" customHeight="1" ht="18">
+      <c r="X98">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" customHeight="1" ht="18">
       <c r="A99" s="12">
         <v>9783</v>
       </c>
@@ -7469,11 +7469,11 @@
         <v>1</v>
       </c>
       <c r="V99" s="12"/>
-      <c r="W99">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="100" spans="1:23" customHeight="1" ht="18">
+      <c r="X99">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" customHeight="1" ht="18">
       <c r="A100" s="12">
         <v>9784</v>
       </c>
@@ -7526,11 +7526,11 @@
         <v>1</v>
       </c>
       <c r="V100" s="12"/>
-      <c r="W100">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="101" spans="1:23" customHeight="1" ht="18">
+      <c r="X100">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" customHeight="1" ht="18">
       <c r="A101" s="12">
         <v>9785</v>
       </c>
@@ -7583,11 +7583,11 @@
         <v>1</v>
       </c>
       <c r="V101" s="12"/>
-      <c r="W101">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="102" spans="1:23" customHeight="1" ht="18">
+      <c r="X101">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" customHeight="1" ht="18">
       <c r="A102" s="12">
         <v>9786</v>
       </c>
@@ -7640,11 +7640,11 @@
         <v>1</v>
       </c>
       <c r="V102" s="12"/>
-      <c r="W102">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="103" spans="1:23" customHeight="1" ht="18">
+      <c r="X102">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" customHeight="1" ht="18">
       <c r="A103" s="12">
         <v>9787</v>
       </c>
@@ -7697,11 +7697,11 @@
         <v>1</v>
       </c>
       <c r="V103" s="12"/>
-      <c r="W103">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="104" spans="1:23" customHeight="1" ht="18">
+      <c r="X103">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" customHeight="1" ht="18">
       <c r="A104" s="12">
         <v>9788</v>
       </c>
@@ -7754,11 +7754,11 @@
         <v>1</v>
       </c>
       <c r="V104" s="12"/>
-      <c r="W104">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="105" spans="1:23" customHeight="1" ht="18">
+      <c r="X104">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" customHeight="1" ht="18">
       <c r="A105" s="12">
         <v>9789</v>
       </c>
@@ -7811,11 +7811,11 @@
         <v>1</v>
       </c>
       <c r="V105" s="12"/>
-      <c r="W105">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="106" spans="1:23" customHeight="1" ht="18">
+      <c r="X105">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" customHeight="1" ht="18">
       <c r="A106" s="12">
         <v>9790</v>
       </c>
@@ -7866,11 +7866,11 @@
         <v>1</v>
       </c>
       <c r="V106" s="12"/>
-      <c r="W106">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="107" spans="1:23" customHeight="1" ht="18">
+      <c r="X106">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" customHeight="1" ht="18">
       <c r="A107" s="12">
         <v>9791</v>
       </c>
@@ -7923,11 +7923,11 @@
         <v>1</v>
       </c>
       <c r="V107" s="12"/>
-      <c r="W107">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="108" spans="1:23" customHeight="1" ht="18">
+      <c r="X107">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" customHeight="1" ht="18">
       <c r="A108" s="12">
         <v>9792</v>
       </c>
@@ -7980,11 +7980,11 @@
         <v>1</v>
       </c>
       <c r="V108" s="12"/>
-      <c r="W108">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="109" spans="1:23" customHeight="1" ht="18">
+      <c r="X108">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" customHeight="1" ht="18">
       <c r="A109" s="12">
         <v>9793</v>
       </c>
@@ -8035,11 +8035,11 @@
         <v>1</v>
       </c>
       <c r="V109" s="12"/>
-      <c r="W109">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="110" spans="1:23" customHeight="1" ht="18">
+      <c r="X109">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" customHeight="1" ht="18">
       <c r="A110" s="12">
         <v>9794</v>
       </c>
@@ -8092,11 +8092,11 @@
         <v>1</v>
       </c>
       <c r="V110" s="12"/>
-      <c r="W110">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="111" spans="1:23" customHeight="1" ht="18">
+      <c r="X110">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" customHeight="1" ht="18">
       <c r="A111" s="12">
         <v>9795</v>
       </c>
@@ -8149,11 +8149,11 @@
         <v>1</v>
       </c>
       <c r="V111" s="12"/>
-      <c r="W111">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="112" spans="1:23" customHeight="1" ht="18">
+      <c r="X111">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="112" spans="1:24" customHeight="1" ht="18">
       <c r="A112" s="12">
         <v>9796</v>
       </c>
@@ -8206,11 +8206,11 @@
         <v>1</v>
       </c>
       <c r="V112" s="12"/>
-      <c r="W112">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="113" spans="1:23" customHeight="1" ht="18">
+      <c r="X112">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" customHeight="1" ht="18">
       <c r="A113" s="12">
         <v>9797</v>
       </c>
@@ -8263,11 +8263,11 @@
         <v>1</v>
       </c>
       <c r="V113" s="12"/>
-      <c r="W113">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="114" spans="1:23" customHeight="1" ht="18">
+      <c r="X113">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" customHeight="1" ht="18">
       <c r="A114" s="12">
         <v>9798</v>
       </c>
@@ -8318,11 +8318,11 @@
         <v>1</v>
       </c>
       <c r="V114" s="12"/>
-      <c r="W114">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="115" spans="1:23" customHeight="1" ht="18">
+      <c r="X114">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" customHeight="1" ht="18">
       <c r="A115" s="12">
         <v>9799</v>
       </c>
@@ -8373,11 +8373,11 @@
         <v>1</v>
       </c>
       <c r="V115" s="12"/>
-      <c r="W115">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="116" spans="1:23" customHeight="1" ht="18">
+      <c r="X115">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" customHeight="1" ht="18">
       <c r="A116" s="12">
         <v>9800</v>
       </c>
@@ -8430,11 +8430,11 @@
         <v>1</v>
       </c>
       <c r="V116" s="12"/>
-      <c r="W116">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="117" spans="1:23" customHeight="1" ht="18">
+      <c r="X116">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" customHeight="1" ht="18">
       <c r="A117" s="12">
         <v>9801</v>
       </c>
@@ -8485,11 +8485,11 @@
         <v>1</v>
       </c>
       <c r="V117" s="12"/>
-      <c r="W117">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="118" spans="1:23" customHeight="1" ht="18">
+      <c r="X117">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" customHeight="1" ht="18">
       <c r="A118" s="12">
         <v>9802</v>
       </c>
@@ -8540,11 +8540,11 @@
         <v>1</v>
       </c>
       <c r="V118" s="12"/>
-      <c r="W118">
-        <v>2070</v>
-      </c>
-    </row>
-    <row r="119" spans="1:23" customHeight="1" ht="18">
+      <c r="X118">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" customHeight="1" ht="18">
       <c r="A119" s="12">
         <v>9803</v>
       </c>
@@ -8597,8 +8597,8 @@
         <v>1</v>
       </c>
       <c r="V119" s="12"/>
-      <c r="W119">
-        <v>2070</v>
+      <c r="X119">
+        <v>2041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>